<commit_message>
Implement manual edit logging feature multiple fixes for feedback until 11/24
</commit_message>
<xml_diff>
--- a/report_template/aggregateReport.xlsx
+++ b/report_template/aggregateReport.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -560,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -568,73 +568,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>

</xml_diff>